<commit_message>
updating based on Sugar Issues
</commit_message>
<xml_diff>
--- a/Templates/Test Plan Template .xlsx
+++ b/Templates/Test Plan Template .xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub_v2\WIP\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646D747A-26FE-40FE-8C8B-BCDD605274D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94803A6F-5814-4FA3-AD42-D0985877CBA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="1680" windowWidth="21600" windowHeight="13740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="40" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Test Case #</t>
   </si>
@@ -129,33 +129,6 @@
   </si>
   <si>
     <t>Justin Pope - 2023-09-27</t>
-  </si>
-  <si>
-    <t>Testing below</t>
-  </si>
-  <si>
-    <t>The following shows that the DeliveryInfo column has been mapped for the delivery phone number</t>
-  </si>
-  <si>
-    <t>Also values that were being populated for the ShipDescription were too long</t>
-  </si>
-  <si>
-    <t>As for the issue for this problem data validation has been made to confirm that the values returned are not causing this issue. The following has been identified:</t>
-  </si>
-  <si>
-    <t>ShippingDescription</t>
-  </si>
-  <si>
-    <t>DeliveryPhoneNumber</t>
-  </si>
-  <si>
-    <t>addressing these issue the test query executes with no issues</t>
-  </si>
-  <si>
-    <t>The solution I am opting for is that of  casting the DeliveryInfo due to the following query of data</t>
-  </si>
-  <si>
-    <t>narrowing the data down to the last few months</t>
   </si>
 </sst>
 </file>
@@ -313,55 +286,55 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -379,231 +352,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>2706399</xdr:colOff>
-      <xdr:row>56</xdr:row>
-      <xdr:rowOff>38339</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A042821A-135F-D474-6903-6244801E2435}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="76200" y="9391650"/>
-          <a:ext cx="9307224" cy="1714739"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>544318</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>1062</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Picture 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9FC5455-2D53-C7E2-C036-D9BA39CE2D5F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="95250" y="3943350"/>
-          <a:ext cx="9983593" cy="7611537"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>601476</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>143935</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Picture 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BAAB2F32-AA82-2835-683B-87040CF5015C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="95250" y="13011150"/>
-          <a:ext cx="10040751" cy="7592485"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>506213</xdr:colOff>
-      <xdr:row>128</xdr:row>
-      <xdr:rowOff>105083</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="Picture 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3664D49-9B3C-E312-3734-1DCB33FFEF11}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="95250" y="21269325"/>
-          <a:ext cx="9945488" cy="2210108"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>131</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>172791</xdr:colOff>
-      <xdr:row>138</xdr:row>
-      <xdr:rowOff>19211</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="9" name="Picture 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE33A51-8D36-EBB6-F5D6-8CAC50BFCE5A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="95250" y="23860125"/>
-          <a:ext cx="9612066" cy="1152686"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -895,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -941,11 +689,11 @@
       <c r="E2" s="13"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="A3" s="16"/>
+      <c r="B3" s="16"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
@@ -957,49 +705,49 @@
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="18"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="20"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="15"/>
+      <c r="B6" s="19"/>
       <c r="C6" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="15"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="15"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="5"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="A9" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="15"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
     </row>
     <row r="10" spans="1:5" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
@@ -1011,49 +759,56 @@
       <c r="E10" s="21"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
-      <c r="E11" s="19"/>
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="17"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>1</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="22"/>
-      <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
+      <c r="C12" s="18"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="18"/>
     </row>
     <row r="13" spans="1:5" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
         <v>2</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
         <v>3</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="A11:E11"/>
     <mergeCell ref="B13:E13"/>
     <mergeCell ref="B14:E14"/>
@@ -1063,13 +818,6 @@
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="B10:E10"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="A5:E5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1081,11 +829,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1100,58 +848,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="22">
+      <c r="B2" s="28"/>
+      <c r="C2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="22" t="str">
+      <c r="B3" s="28"/>
+      <c r="C3" s="18" t="str">
         <f>'Test Cases'!B2</f>
         <v>Unit Testing</v>
       </c>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" ht="57.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="22" t="str">
+      <c r="B4" s="28"/>
+      <c r="C4" s="18" t="str">
         <f>'Test Cases'!D2</f>
         <v xml:space="preserve">1) </v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="28"/>
-      <c r="C5" s="28"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
       <c r="D5" s="14" t="s">
         <v>19</v>
       </c>
@@ -1163,103 +911,69 @@
       </c>
     </row>
     <row r="6" spans="1:6" s="10" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
     </row>
     <row r="7" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="13" t="s">
-        <v>31</v>
-      </c>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="25"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
     </row>
     <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
     </row>
     <row r="10" spans="1:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="19"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="1:6" ht="99.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="24"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-    </row>
-    <row r="45" spans="3:4" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C45" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="60" spans="3:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="C60" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C61" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C62" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="64" spans="3:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C64" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="115" spans="3:3" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="C115" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="131" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C131" s="3" t="s">
-        <v>39</v>
-      </c>
+      <c r="A11" s="31"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+    </row>
+    <row r="45" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D45" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A11:F11"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A10:F10"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A8:F8"/>
@@ -1271,19 +985,28 @@
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:F3"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A11:F11"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:F10"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="5" scale="94" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="1a638d2c-e7c0-419c-9191-e92086f67d97">
@@ -1292,19 +1015,6 @@
     <TaxCatchAll xmlns="84e25877-5f26-4dc3-9598-48e40fb4ec5c" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1539,12 +1249,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1336CC8-439A-433F-AFCD-D3738BD4CF84}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433CEB9C-4DCB-4DF9-8E44-99AD43459D1C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="84e25877-5f26-4dc3-9598-48e40fb4ec5c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1558,9 +1265,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{433CEB9C-4DCB-4DF9-8E44-99AD43459D1C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D1336CC8-439A-433F-AFCD-D3738BD4CF84}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1a638d2c-e7c0-419c-9191-e92086f67d97"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="84e25877-5f26-4dc3-9598-48e40fb4ec5c"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>